<commit_message>
stuff done i class workshop2
</commit_message>
<xml_diff>
--- a/data/PROJEKTSHEETV2.0.xlsx
+++ b/data/PROJEKTSHEETV2.0.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Emma-Marie/Documents/AU/ka_2.semester/rel_projekt/rel_projekt/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Emma-Marie/Documents/AU/ka_2.semester/rel_projekt/rel_projekt/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2746B94D-3A31-D242-A481-605A251C86D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B451CECA-0A05-F54B-9C3C-4F55219462EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15840" xr2:uid="{36EF6E76-F446-4A76-BCD5-6E706DA0D5A2}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="27160" windowHeight="15840" xr2:uid="{36EF6E76-F446-4A76-BCD5-6E706DA0D5A2}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="179">
   <si>
     <t>STUDENT</t>
   </si>
@@ -559,6 +559,24 @@
   </si>
   <si>
     <t>Mekka</t>
+  </si>
+  <si>
+    <t>Emma</t>
+  </si>
+  <si>
+    <t>home</t>
+  </si>
+  <si>
+    <t>Projektingeniør</t>
+  </si>
+  <si>
+    <t>dansk-islandsk</t>
+  </si>
+  <si>
+    <t>sf</t>
+  </si>
+  <si>
+    <t>folkekirken</t>
   </si>
 </sst>
 </file>
@@ -948,8 +966,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1642A8C-A2FE-4D62-8416-8B05C6783932}">
   <dimension ref="A1:EK7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="172" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="BH1" zoomScale="172" workbookViewId="0">
+      <selection activeCell="AY11" sqref="AY11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1875,6 +1893,419 @@
         <v>10</v>
       </c>
       <c r="G5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:141" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>173</v>
+      </c>
+      <c r="C6" s="1">
+        <v>45553</v>
+      </c>
+      <c r="D6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" t="s">
+        <v>174</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <v>28</v>
+      </c>
+      <c r="J6" t="s">
+        <v>175</v>
+      </c>
+      <c r="L6" t="s">
+        <v>176</v>
+      </c>
+      <c r="M6">
+        <v>6</v>
+      </c>
+      <c r="N6">
+        <v>16</v>
+      </c>
+      <c r="O6">
+        <v>2</v>
+      </c>
+      <c r="P6">
+        <v>28</v>
+      </c>
+      <c r="Q6">
+        <v>1</v>
+      </c>
+      <c r="R6">
+        <v>-2</v>
+      </c>
+      <c r="S6">
+        <v>1</v>
+      </c>
+      <c r="T6">
+        <v>0</v>
+      </c>
+      <c r="U6">
+        <v>1</v>
+      </c>
+      <c r="V6">
+        <v>1</v>
+      </c>
+      <c r="W6">
+        <v>0</v>
+      </c>
+      <c r="X6">
+        <v>5</v>
+      </c>
+      <c r="Y6">
+        <v>2</v>
+      </c>
+      <c r="Z6">
+        <v>1</v>
+      </c>
+      <c r="AA6">
+        <v>-1</v>
+      </c>
+      <c r="AB6" t="s">
+        <v>177</v>
+      </c>
+      <c r="AC6">
+        <v>1</v>
+      </c>
+      <c r="AD6">
+        <v>-1</v>
+      </c>
+      <c r="AE6">
+        <v>-1</v>
+      </c>
+      <c r="AF6">
+        <v>0</v>
+      </c>
+      <c r="AG6">
+        <v>2</v>
+      </c>
+      <c r="AH6">
+        <v>1</v>
+      </c>
+      <c r="AI6">
+        <v>1</v>
+      </c>
+      <c r="AJ6">
+        <v>-1</v>
+      </c>
+      <c r="AK6">
+        <v>0</v>
+      </c>
+      <c r="AL6">
+        <v>0</v>
+      </c>
+      <c r="AM6">
+        <v>0</v>
+      </c>
+      <c r="AN6">
+        <v>-1</v>
+      </c>
+      <c r="AO6">
+        <v>-2</v>
+      </c>
+      <c r="AP6">
+        <v>-2</v>
+      </c>
+      <c r="AQ6">
+        <v>-2</v>
+      </c>
+      <c r="AR6">
+        <v>-2</v>
+      </c>
+      <c r="AS6">
+        <v>-2</v>
+      </c>
+      <c r="AT6">
+        <v>-1</v>
+      </c>
+      <c r="AU6">
+        <v>0</v>
+      </c>
+      <c r="AV6">
+        <v>0</v>
+      </c>
+      <c r="AW6">
+        <v>-2</v>
+      </c>
+      <c r="AX6">
+        <v>-1</v>
+      </c>
+      <c r="AY6">
+        <v>1</v>
+      </c>
+      <c r="AZ6">
+        <v>-2</v>
+      </c>
+      <c r="BA6">
+        <v>0</v>
+      </c>
+      <c r="BB6">
+        <v>-1</v>
+      </c>
+      <c r="BC6">
+        <v>-1</v>
+      </c>
+      <c r="BD6">
+        <v>-2</v>
+      </c>
+      <c r="BE6">
+        <v>0</v>
+      </c>
+      <c r="BF6">
+        <v>-2</v>
+      </c>
+      <c r="BG6">
+        <v>0</v>
+      </c>
+      <c r="BH6">
+        <v>1</v>
+      </c>
+      <c r="BI6">
+        <v>1</v>
+      </c>
+      <c r="BJ6">
+        <v>1</v>
+      </c>
+      <c r="BK6">
+        <v>1</v>
+      </c>
+      <c r="BL6" t="s">
+        <v>178</v>
+      </c>
+      <c r="BM6">
+        <v>0</v>
+      </c>
+      <c r="BN6">
+        <v>0</v>
+      </c>
+      <c r="BO6">
+        <v>0</v>
+      </c>
+      <c r="BP6">
+        <v>999</v>
+      </c>
+      <c r="BQ6">
+        <v>0</v>
+      </c>
+      <c r="BR6">
+        <v>0</v>
+      </c>
+      <c r="BS6">
+        <v>0</v>
+      </c>
+      <c r="BT6">
+        <v>0</v>
+      </c>
+      <c r="BU6">
+        <v>1</v>
+      </c>
+      <c r="BV6">
+        <v>1</v>
+      </c>
+      <c r="BW6">
+        <v>3</v>
+      </c>
+      <c r="BX6">
+        <v>-1</v>
+      </c>
+      <c r="BY6">
+        <v>0</v>
+      </c>
+      <c r="BZ6">
+        <v>-2</v>
+      </c>
+      <c r="CA6">
+        <v>-2</v>
+      </c>
+      <c r="CB6">
+        <v>-1</v>
+      </c>
+      <c r="CC6">
+        <v>-2</v>
+      </c>
+      <c r="CD6">
+        <v>-2</v>
+      </c>
+      <c r="CE6">
+        <v>-2</v>
+      </c>
+      <c r="CF6">
+        <v>-2</v>
+      </c>
+      <c r="CG6">
+        <v>0</v>
+      </c>
+      <c r="CH6">
+        <v>0</v>
+      </c>
+      <c r="CI6">
+        <v>-2</v>
+      </c>
+      <c r="CJ6">
+        <v>-2</v>
+      </c>
+      <c r="CK6">
+        <v>1</v>
+      </c>
+      <c r="CL6">
+        <v>-1</v>
+      </c>
+      <c r="CM6">
+        <v>1</v>
+      </c>
+      <c r="CN6">
+        <v>-2</v>
+      </c>
+      <c r="CO6">
+        <v>-2</v>
+      </c>
+      <c r="CP6">
+        <v>-2</v>
+      </c>
+      <c r="CQ6">
+        <v>0</v>
+      </c>
+      <c r="CR6">
+        <v>-2</v>
+      </c>
+      <c r="CS6">
+        <v>0</v>
+      </c>
+      <c r="CT6">
+        <v>1</v>
+      </c>
+      <c r="CU6">
+        <v>-2</v>
+      </c>
+      <c r="CV6">
+        <v>-2</v>
+      </c>
+      <c r="CW6">
+        <v>-2</v>
+      </c>
+      <c r="CX6">
+        <v>-2</v>
+      </c>
+      <c r="CY6">
+        <v>-2</v>
+      </c>
+      <c r="CZ6">
+        <v>1</v>
+      </c>
+      <c r="DA6">
+        <v>-2</v>
+      </c>
+      <c r="DB6">
+        <v>1</v>
+      </c>
+      <c r="DC6">
+        <v>-2</v>
+      </c>
+      <c r="DD6">
+        <v>-2</v>
+      </c>
+      <c r="DE6">
+        <v>-2</v>
+      </c>
+      <c r="DF6">
+        <v>-2</v>
+      </c>
+      <c r="DG6">
+        <v>-2</v>
+      </c>
+      <c r="DH6">
+        <v>-2</v>
+      </c>
+      <c r="DI6">
+        <v>-2</v>
+      </c>
+      <c r="DJ6">
+        <v>-2</v>
+      </c>
+      <c r="DK6">
+        <v>-2</v>
+      </c>
+      <c r="DL6">
+        <v>-2</v>
+      </c>
+      <c r="DM6">
+        <v>-2</v>
+      </c>
+      <c r="DN6">
+        <v>-2</v>
+      </c>
+      <c r="DO6">
+        <v>-2</v>
+      </c>
+      <c r="DP6">
+        <v>-2</v>
+      </c>
+      <c r="DQ6">
+        <v>1</v>
+      </c>
+      <c r="DR6">
+        <v>1</v>
+      </c>
+      <c r="DS6">
+        <v>-2</v>
+      </c>
+      <c r="DT6">
+        <v>0</v>
+      </c>
+      <c r="DU6">
+        <v>-2</v>
+      </c>
+      <c r="DV6">
+        <v>1</v>
+      </c>
+      <c r="DW6">
+        <v>0</v>
+      </c>
+      <c r="DX6">
+        <v>-2</v>
+      </c>
+      <c r="DY6">
+        <v>-2</v>
+      </c>
+      <c r="DZ6">
+        <v>2</v>
+      </c>
+      <c r="EA6">
+        <v>1</v>
+      </c>
+      <c r="EB6">
+        <v>-2</v>
+      </c>
+      <c r="EC6">
+        <v>0</v>
+      </c>
+      <c r="ED6">
+        <v>-2</v>
+      </c>
+      <c r="EE6">
+        <v>-2</v>
+      </c>
+      <c r="EF6">
+        <v>-2</v>
+      </c>
+      <c r="EG6">
+        <v>-2</v>
+      </c>
+      <c r="EH6">
+        <v>-2</v>
+      </c>
+      <c r="EI6">
+        <v>-2</v>
+      </c>
+      <c r="EJ6">
         <v>1</v>
       </c>
     </row>

</xml_diff>